<commit_message>
betting data week 16
</commit_message>
<xml_diff>
--- a/data/external/NFL Bets.xlsx
+++ b/data/external/NFL Bets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johno\Documents\Sports Research\NFL\data\external\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johno\Documents\nfl-dashboard\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400DEEE8-2176-4021-B15D-F42F1D572CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDAFF42-62BF-412A-8D7C-E1379360C6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="615" windowWidth="15840" windowHeight="13950" activeTab="3" xr2:uid="{D3456828-AB8A-415C-A83D-57D4898B5C22}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="3" xr2:uid="{D3456828-AB8A-415C-A83D-57D4898B5C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 13" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="218">
   <si>
     <t>Placed</t>
   </si>
@@ -688,6 +688,18 @@
   </si>
   <si>
     <t>Devaugn Vele First Touchdown Scorer</t>
+  </si>
+  <si>
+    <t>Zay Flowers Over 63.5 Receiving Yards</t>
+  </si>
+  <si>
+    <t>Deebo Samuel ATTD</t>
+  </si>
+  <si>
+    <t>Zay Flowers Over 73.5 Receiving Yards</t>
+  </si>
+  <si>
+    <t>Zay Flowers Over 133.5 Receiving Yards</t>
   </si>
 </sst>
 </file>
@@ -897,7 +909,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -945,11 +957,34 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="85">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
@@ -1125,26 +1160,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2347,7 +2362,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{640518E4-06CF-42A5-B915-D490AECF8A4F}" name="Table410" displayName="Table410" ref="N1:N2" totalsRowShown="0">
   <autoFilter ref="N1:N2" xr:uid="{640518E4-06CF-42A5-B915-D490AECF8A4F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B54B31F5-F845-4F81-8504-211808C65E33}" name="Overall" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{B54B31F5-F845-4F81-8504-211808C65E33}" name="Overall" dataDxfId="16">
       <calculatedColumnFormula>SUM(J2:J43)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2359,7 +2374,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{20C120D7-188C-4B5D-AE18-55DA1D939103}" name="Table411" displayName="Table411" ref="N1:N2" totalsRowShown="0">
   <autoFilter ref="N1:N2" xr:uid="{20C120D7-188C-4B5D-AE18-55DA1D939103}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{57354695-8883-4AD9-B220-FDD51F55C90F}" name="Overall" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{57354695-8883-4AD9-B220-FDD51F55C90F}" name="Overall" dataDxfId="15">
       <calculatedColumnFormula>SUM(J2:J43)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2371,7 +2386,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{85A3BD06-E8DF-4487-B087-FE5AC251BB90}" name="Table412" displayName="Table412" ref="N1:N2" totalsRowShown="0">
   <autoFilter ref="N1:N2" xr:uid="{85A3BD06-E8DF-4487-B087-FE5AC251BB90}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C407F22F-7145-49D7-9996-A169C2F4889E}" name="Overall" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{C407F22F-7145-49D7-9996-A169C2F4889E}" name="Overall" dataDxfId="14">
       <calculatedColumnFormula>SUM(J2:J43)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2383,7 +2398,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{9D399345-24BB-4D5C-ACA8-43292826CF4E}" name="Table413" displayName="Table413" ref="N1:N2" totalsRowShown="0">
   <autoFilter ref="N1:N2" xr:uid="{9D399345-24BB-4D5C-ACA8-43292826CF4E}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{BFB8A5CC-B418-495E-99FF-1CC4E3749EE2}" name="Overall" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{BFB8A5CC-B418-495E-99FF-1CC4E3749EE2}" name="Overall" dataDxfId="13">
       <calculatedColumnFormula>SUM(J2:J43)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2395,7 +2410,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{773EEAB1-ADB0-40CC-849B-DD43A324357F}" name="Table414" displayName="Table414" ref="N1:N2" totalsRowShown="0">
   <autoFilter ref="N1:N2" xr:uid="{773EEAB1-ADB0-40CC-849B-DD43A324357F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3D62CFB2-BB61-41FC-9050-FA22D1A931F2}" name="Overall" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{3D62CFB2-BB61-41FC-9050-FA22D1A931F2}" name="Overall" dataDxfId="12">
       <calculatedColumnFormula>SUM(J2:J43)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2404,20 +2419,20 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{885B85B5-C73C-4ECF-99B3-7DF99C7AA09E}" name="Table2" displayName="Table2" ref="A1:I19" totalsRowShown="0" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{885B85B5-C73C-4ECF-99B3-7DF99C7AA09E}" name="Table2" displayName="Table2" ref="A1:I19" totalsRowShown="0" dataDxfId="11">
   <autoFilter ref="A1:I19" xr:uid="{885B85B5-C73C-4ECF-99B3-7DF99C7AA09E}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{CF99D162-A6B9-45EC-9A0A-4FC785FF5A38}" name="Placed" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{1672D3B9-B813-4537-823C-20F5B31EBA4C}" name="Sportsbook" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{6E910389-FFE7-47EE-95C2-21A2191A0F9F}" name="Type" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{2C6487B9-073D-4AE2-A82A-4FC1FF2EAEF5}" name="Description" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{20FB75B1-5466-4E6E-82FA-E5816870E041}" name="Odds" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{3A7F6EFB-86B1-4522-B378-CF85170E300A}" name="Wager" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{8453FE5D-0944-4E82-9B2E-899F833A8B7E}" name="Payout" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{CF99D162-A6B9-45EC-9A0A-4FC785FF5A38}" name="Placed" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{1672D3B9-B813-4537-823C-20F5B31EBA4C}" name="Sportsbook" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{6E910389-FFE7-47EE-95C2-21A2191A0F9F}" name="Type" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{2C6487B9-073D-4AE2-A82A-4FC1FF2EAEF5}" name="Description" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{20FB75B1-5466-4E6E-82FA-E5816870E041}" name="Odds" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{3A7F6EFB-86B1-4522-B378-CF85170E300A}" name="Wager" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{8453FE5D-0944-4E82-9B2E-899F833A8B7E}" name="Payout" dataDxfId="4">
       <calculatedColumnFormula>IF(E2 &gt; 0, F2 * (E2 / 100), F2 * (100 / ABS(E2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{BFF6A3EE-AAFF-49E3-B181-859025AA5503}" name="Result" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{03A83778-D830-4DB2-B844-E08D5408FB84}" name="Net" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{BFF6A3EE-AAFF-49E3-B181-859025AA5503}" name="Result" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{03A83778-D830-4DB2-B844-E08D5408FB84}" name="Net" dataDxfId="2">
       <calculatedColumnFormula>IF(H2="", "", IF(H2="Win", G2, -F2))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2429,7 +2444,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{57D8DD86-0B0D-47A6-BAD6-B3E780AF986B}" name="Table415" displayName="Table415" ref="K1:K2" totalsRowShown="0">
   <autoFilter ref="K1:K2" xr:uid="{57D8DD86-0B0D-47A6-BAD6-B3E780AF986B}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{E4B92AD6-C951-4977-ADAB-D4DAD2B54B91}" name="Overall" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{E4B92AD6-C951-4977-ADAB-D4DAD2B54B91}" name="Overall" dataDxfId="1">
       <calculatedColumnFormula>SUM(I2:I19)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2534,7 +2549,7 @@
   <autoFilter ref="N1:N2" xr:uid="{43AEE642-1FFB-47A4-860A-B5F46F452064}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{5619EDB5-6C54-404D-A7CB-2926D193E89C}" name="Overall" dataDxfId="34">
-      <calculatedColumnFormula>SUM(J2:J30)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(J2:J29)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2542,8 +2557,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{AFA2B4A0-DB38-432A-9026-4AB1B57E4E84}" name="Table15" displayName="Table15" ref="A1:L19" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
-  <autoFilter ref="A1:L19" xr:uid="{AFA2B4A0-DB38-432A-9026-4AB1B57E4E84}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{AFA2B4A0-DB38-432A-9026-4AB1B57E4E84}" name="Table15" displayName="Table15" ref="A1:L21" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+  <autoFilter ref="A1:L21" xr:uid="{AFA2B4A0-DB38-432A-9026-4AB1B57E4E84}">
+    <filterColumn colId="3">
+      <filters blank="1">
+        <filter val="ARI @ CAR"/>
+        <filter val="DET @ CHI"/>
+        <filter val="HOU @ KC"/>
+        <filter val="Multiple"/>
+        <filter val="NYJ @ LAR"/>
+        <filter val="PIT @ BAL"/>
+        <filter val="SF @ MIA"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{45ECF88B-29E2-4121-B242-BFC135968440}" name="Placed" dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{9F2D627C-4831-4AEA-A4E8-1FB28B6F41A5}" name="Sportsbook" dataDxfId="27"/>
@@ -2556,9 +2583,11 @@
       <calculatedColumnFormula>IF(F2 &gt; 0, G2 * (F2 / 100), G2 * (100 / ABS(F2)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{9ABE133E-7E00-450D-A148-57A75D61B199}" name="Result" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{672202F6-F312-45B0-95E5-85CD7B072CC0}" name="Net" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{E386B0E7-13C5-442B-9332-11DE838696AC}" name="Bet Result" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{6BA4F692-9676-4373-A5DD-6D818094A615}" name="Notes" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{672202F6-F312-45B0-95E5-85CD7B072CC0}" name="Net" dataDxfId="0">
+      <calculatedColumnFormula>IF(I2="", "", IF(I2="Win", H2, -G2))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{E386B0E7-13C5-442B-9332-11DE838696AC}" name="Bet Result" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{6BA4F692-9676-4373-A5DD-6D818094A615}" name="Notes" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2568,7 +2597,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{813C3E68-16D4-4AC3-A533-C116E1127B25}" name="Table49" displayName="Table49" ref="N1:N2" totalsRowShown="0">
   <autoFilter ref="N1:N2" xr:uid="{813C3E68-16D4-4AC3-A533-C116E1127B25}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3E3EE77D-5FAB-449B-ADA5-AA0BC5D7434C}" name="Overall" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{3E3EE77D-5FAB-449B-ADA5-AA0BC5D7434C}" name="Overall" dataDxfId="17">
       <calculatedColumnFormula>SUM(J2:J43)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2899,22 +2928,22 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2955,7 +2984,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45624</v>
       </c>
@@ -2997,7 +3026,7 @@
         <v>90.412558578733993</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45623</v>
       </c>
@@ -3035,7 +3064,7 @@
       </c>
       <c r="L3" s="34"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45624</v>
       </c>
@@ -3073,7 +3102,7 @@
       </c>
       <c r="L4" s="34"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45624</v>
       </c>
@@ -3111,7 +3140,7 @@
       </c>
       <c r="L5" s="34"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45622</v>
       </c>
@@ -3149,7 +3178,7 @@
       </c>
       <c r="L6" s="34"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45622</v>
       </c>
@@ -3187,7 +3216,7 @@
       </c>
       <c r="L7" s="34"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45622</v>
       </c>
@@ -3225,7 +3254,7 @@
       </c>
       <c r="L8" s="34"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45622</v>
       </c>
@@ -3263,7 +3292,7 @@
       </c>
       <c r="L9" s="34"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45624</v>
       </c>
@@ -3301,7 +3330,7 @@
       </c>
       <c r="L10" s="34"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45621</v>
       </c>
@@ -3339,7 +3368,7 @@
       </c>
       <c r="L11" s="34"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45621</v>
       </c>
@@ -3377,7 +3406,7 @@
       </c>
       <c r="L12" s="34"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45623</v>
       </c>
@@ -3415,7 +3444,7 @@
       </c>
       <c r="L13" s="34"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45622</v>
       </c>
@@ -3453,7 +3482,7 @@
       </c>
       <c r="L14" s="34"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45623</v>
       </c>
@@ -3491,7 +3520,7 @@
       </c>
       <c r="L15" s="34"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45622</v>
       </c>
@@ -3529,7 +3558,7 @@
       </c>
       <c r="L16" s="34"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45625</v>
       </c>
@@ -3567,7 +3596,7 @@
       </c>
       <c r="L17" s="34"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45625</v>
       </c>
@@ -3607,7 +3636,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45624</v>
       </c>
@@ -3645,7 +3674,7 @@
       </c>
       <c r="L19" s="34"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45623</v>
       </c>
@@ -3683,7 +3712,7 @@
       </c>
       <c r="L20" s="34"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45622</v>
       </c>
@@ -3721,7 +3750,7 @@
       </c>
       <c r="L21" s="34"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45622</v>
       </c>
@@ -3759,7 +3788,7 @@
       </c>
       <c r="L22" s="34"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45622</v>
       </c>
@@ -3797,7 +3826,7 @@
       </c>
       <c r="L23" s="34"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45621</v>
       </c>
@@ -3835,7 +3864,7 @@
       </c>
       <c r="L24" s="34"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45624</v>
       </c>
@@ -3873,7 +3902,7 @@
       </c>
       <c r="L25" s="34"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45624</v>
       </c>
@@ -3911,7 +3940,7 @@
       </c>
       <c r="L26" s="34"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45623</v>
       </c>
@@ -3949,7 +3978,7 @@
       </c>
       <c r="L27" s="34"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45623</v>
       </c>
@@ -3987,7 +4016,7 @@
       </c>
       <c r="L28" s="34"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45622</v>
       </c>
@@ -4025,7 +4054,7 @@
       </c>
       <c r="L29" s="34"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45622</v>
       </c>
@@ -4063,7 +4092,7 @@
       </c>
       <c r="L30" s="34"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45622</v>
       </c>
@@ -4101,7 +4130,7 @@
       </c>
       <c r="L31" s="34"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45623</v>
       </c>
@@ -4139,7 +4168,7 @@
       </c>
       <c r="L32" s="34"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>45623</v>
       </c>
@@ -4177,7 +4206,7 @@
       </c>
       <c r="L33" s="34"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>45622</v>
       </c>
@@ -4215,7 +4244,7 @@
       </c>
       <c r="L34" s="34"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>45622</v>
       </c>
@@ -4253,7 +4282,7 @@
       </c>
       <c r="L35" s="34"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>45622</v>
       </c>
@@ -4291,7 +4320,7 @@
       </c>
       <c r="L36" s="34"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>45621</v>
       </c>
@@ -4329,7 +4358,7 @@
       </c>
       <c r="L37" s="34"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>45622</v>
       </c>
@@ -4367,7 +4396,7 @@
       </c>
       <c r="L38" s="34"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>45628</v>
       </c>
@@ -4405,7 +4434,7 @@
       </c>
       <c r="L39" s="34"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>45628</v>
       </c>
@@ -4443,7 +4472,7 @@
       </c>
       <c r="L40" s="34"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>45628</v>
       </c>
@@ -4481,7 +4510,7 @@
       </c>
       <c r="L41" s="34"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>45628</v>
       </c>
@@ -4519,7 +4548,7 @@
       </c>
       <c r="L42" s="34"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>45627</v>
       </c>
@@ -4574,9 +4603,9 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4617,7 +4646,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -4638,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -4668,20 +4697,20 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4713,7 +4742,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45524</v>
       </c>
@@ -4746,7 +4775,7 @@
         <v>211.17050691244239</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>45554</v>
       </c>
@@ -4775,7 +4804,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>45607</v>
       </c>
@@ -4804,7 +4833,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>45556</v>
       </c>
@@ -4835,7 +4864,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>45556</v>
       </c>
@@ -4864,7 +4893,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>45556</v>
       </c>
@@ -4893,7 +4922,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>45524</v>
       </c>
@@ -4924,7 +4953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>45532</v>
       </c>
@@ -4955,7 +4984,7 @@
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>45532</v>
       </c>
@@ -4986,7 +5015,7 @@
         <v>28.2258064516129</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>45512</v>
       </c>
@@ -5017,7 +5046,7 @@
         <v>32.258064516129032</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>45512</v>
       </c>
@@ -5048,7 +5077,7 @@
         <v>32.258064516129032</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>45517</v>
       </c>
@@ -5077,7 +5106,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>45517</v>
       </c>
@@ -5106,7 +5135,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>45524</v>
       </c>
@@ -5135,7 +5164,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>45512</v>
       </c>
@@ -5166,7 +5195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>45622</v>
       </c>
@@ -5195,7 +5224,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>45644</v>
       </c>
@@ -5224,7 +5253,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>45644</v>
       </c>
@@ -5270,18 +5299,18 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -5322,7 +5351,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="15">
         <v>45628</v>
       </c>
@@ -5364,7 +5393,7 @@
         <v>54.588788740838218</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>45632</v>
       </c>
@@ -5402,7 +5431,7 @@
       </c>
       <c r="L3" s="16"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>45632</v>
       </c>
@@ -5440,7 +5469,7 @@
       </c>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>45632</v>
       </c>
@@ -5478,7 +5507,7 @@
       </c>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>45632</v>
       </c>
@@ -5516,7 +5545,7 @@
       </c>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>45632</v>
       </c>
@@ -5554,7 +5583,7 @@
       </c>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>45632</v>
       </c>
@@ -5592,7 +5621,7 @@
       </c>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>45632</v>
       </c>
@@ -5630,7 +5659,7 @@
       </c>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>45632</v>
       </c>
@@ -5668,7 +5697,7 @@
       </c>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>45632</v>
       </c>
@@ -5706,7 +5735,7 @@
       </c>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <v>45624</v>
       </c>
@@ -5744,7 +5773,7 @@
       </c>
       <c r="L12" s="16"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>45624</v>
       </c>
@@ -5782,7 +5811,7 @@
       </c>
       <c r="L13" s="16"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>45628</v>
       </c>
@@ -5820,7 +5849,7 @@
       </c>
       <c r="L14" s="19"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>45628</v>
       </c>
@@ -5858,7 +5887,7 @@
       </c>
       <c r="L15" s="19"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>45628</v>
       </c>
@@ -5896,7 +5925,7 @@
       </c>
       <c r="L16" s="19"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>45630</v>
       </c>
@@ -5934,7 +5963,7 @@
       </c>
       <c r="L17" s="19"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>45630</v>
       </c>
@@ -5972,7 +6001,7 @@
       </c>
       <c r="L18" s="16"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>45630</v>
       </c>
@@ -6010,7 +6039,7 @@
       </c>
       <c r="L19" s="16"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>45630</v>
       </c>
@@ -6048,7 +6077,7 @@
       </c>
       <c r="L20" s="19"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>45630</v>
       </c>
@@ -6086,7 +6115,7 @@
       </c>
       <c r="L21" s="19"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <v>45628</v>
       </c>
@@ -6124,7 +6153,7 @@
       </c>
       <c r="L22" s="19"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>45629</v>
       </c>
@@ -6162,7 +6191,7 @@
       </c>
       <c r="L23" s="19"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>45633</v>
       </c>
@@ -6200,7 +6229,7 @@
       </c>
       <c r="L24" s="19"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <v>45632</v>
       </c>
@@ -6238,7 +6267,7 @@
       </c>
       <c r="L25" s="19"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="18">
         <v>45634</v>
       </c>
@@ -6276,7 +6305,7 @@
       </c>
       <c r="L26" s="19"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="18">
         <v>45630</v>
       </c>
@@ -6314,7 +6343,7 @@
       </c>
       <c r="L27" s="19"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="18">
         <v>45630</v>
       </c>
@@ -6352,7 +6381,7 @@
       </c>
       <c r="L28" s="19"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
         <v>45630</v>
       </c>
@@ -6390,7 +6419,7 @@
       </c>
       <c r="L29" s="19"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="18">
         <v>45632</v>
       </c>
@@ -6428,7 +6457,7 @@
       </c>
       <c r="L30" s="19"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="18">
         <v>45632</v>
       </c>
@@ -6466,7 +6495,7 @@
       </c>
       <c r="L31" s="19"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
         <v>45632</v>
       </c>
@@ -6504,7 +6533,7 @@
       </c>
       <c r="L32" s="19"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
         <v>45632</v>
       </c>
@@ -6542,7 +6571,7 @@
       </c>
       <c r="L33" s="19"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="18">
         <v>45628</v>
       </c>
@@ -6580,7 +6609,7 @@
       </c>
       <c r="L34" s="19"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="15">
         <v>45632</v>
       </c>
@@ -6618,7 +6647,7 @@
       </c>
       <c r="L35" s="16"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>45635</v>
       </c>
@@ -6656,7 +6685,7 @@
       </c>
       <c r="L36" s="16"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <v>45635</v>
       </c>
@@ -6694,7 +6723,7 @@
       </c>
       <c r="L37" s="19"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <v>45635</v>
       </c>
@@ -6732,7 +6761,7 @@
       </c>
       <c r="L38" s="19"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <v>45635</v>
       </c>
@@ -6770,7 +6799,7 @@
       </c>
       <c r="L39" s="19"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="15">
         <v>45635</v>
       </c>
@@ -6808,7 +6837,7 @@
       </c>
       <c r="L40" s="16"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="15">
         <v>45635</v>
       </c>
@@ -6846,7 +6875,7 @@
       </c>
       <c r="L41" s="19"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="15">
         <v>45635</v>
       </c>
@@ -6884,7 +6913,7 @@
       </c>
       <c r="L42" s="19"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="15">
         <v>45635</v>
       </c>
@@ -6922,7 +6951,7 @@
       </c>
       <c r="L43" s="19"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>45634</v>
       </c>
@@ -6977,18 +7006,18 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -7029,7 +7058,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="30">
         <v>45635</v>
       </c>
@@ -7059,7 +7088,7 @@
         <v>90</v>
       </c>
       <c r="J2" s="26">
-        <f t="shared" ref="J2:J26" si="1">IF(I2="", "", IF(I2="Win", H2, -G2))</f>
+        <f>IF(I2="", "", IF(I2="Win", H2, -G2))</f>
         <v>18.18181818181818</v>
       </c>
       <c r="K2" s="25">
@@ -7071,7 +7100,7 @@
         <v>-59.508882928665543</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <v>45642</v>
       </c>
@@ -7101,7 +7130,7 @@
         <v>89</v>
       </c>
       <c r="J3" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J2:J26" si="1">IF(I3="", "", IF(I3="Win", H3, -G3))</f>
         <v>-5</v>
       </c>
       <c r="K3" s="32">
@@ -7109,7 +7138,7 @@
       </c>
       <c r="L3" s="32"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>45642</v>
       </c>
@@ -7147,7 +7176,7 @@
       </c>
       <c r="L4" s="25"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>45642</v>
       </c>
@@ -7185,7 +7214,7 @@
       </c>
       <c r="L5" s="25"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>45642</v>
       </c>
@@ -7223,7 +7252,7 @@
       </c>
       <c r="L6" s="25"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>45642</v>
       </c>
@@ -7261,7 +7290,7 @@
       </c>
       <c r="L7" s="25"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
         <v>45640</v>
       </c>
@@ -7299,7 +7328,7 @@
       </c>
       <c r="L8" s="32"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>45642</v>
       </c>
@@ -7337,7 +7366,7 @@
       </c>
       <c r="L9" s="25"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="30">
         <v>45642</v>
       </c>
@@ -7375,7 +7404,7 @@
       </c>
       <c r="L10" s="25"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="30">
         <v>45642</v>
       </c>
@@ -7413,7 +7442,7 @@
       </c>
       <c r="L11" s="25"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="30">
         <v>45642</v>
       </c>
@@ -7451,7 +7480,7 @@
       </c>
       <c r="L12" s="32"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="30">
         <v>45632</v>
       </c>
@@ -7489,7 +7518,7 @@
       </c>
       <c r="L13" s="25"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="30">
         <v>45637</v>
       </c>
@@ -7527,7 +7556,7 @@
       </c>
       <c r="L14" s="32"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="30">
         <v>45638</v>
       </c>
@@ -7565,7 +7594,7 @@
       </c>
       <c r="L15" s="32"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
         <v>45636</v>
       </c>
@@ -7603,7 +7632,7 @@
       </c>
       <c r="L16" s="32"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="30">
         <v>45638</v>
       </c>
@@ -7641,7 +7670,7 @@
       </c>
       <c r="L17" s="25"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="30">
         <v>45638</v>
       </c>
@@ -7679,7 +7708,7 @@
       </c>
       <c r="L18" s="32"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="30">
         <v>45638</v>
       </c>
@@ -7717,7 +7746,7 @@
       </c>
       <c r="L19" s="25"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="30">
         <v>45638</v>
       </c>
@@ -7755,7 +7784,7 @@
       </c>
       <c r="L20" s="32"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="30">
         <v>45638</v>
       </c>
@@ -7793,7 +7822,7 @@
       </c>
       <c r="L21" s="25"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="30">
         <v>45638</v>
       </c>
@@ -7831,7 +7860,7 @@
       </c>
       <c r="L22" s="25"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="30">
         <v>45638</v>
       </c>
@@ -7871,7 +7900,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="30">
         <v>45640</v>
       </c>
@@ -7909,7 +7938,7 @@
       </c>
       <c r="L24" s="25"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="30">
         <v>45641</v>
       </c>
@@ -7947,7 +7976,7 @@
       </c>
       <c r="L25" s="32"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="30">
         <v>45641</v>
       </c>
@@ -7985,7 +8014,7 @@
       </c>
       <c r="L26" s="25"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="30">
         <v>45635</v>
       </c>
@@ -8022,7 +8051,7 @@
       </c>
       <c r="L27" s="25"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="30">
         <v>45636</v>
       </c>
@@ -8060,7 +8089,7 @@
       </c>
       <c r="L28" s="25"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="30">
         <v>45636</v>
       </c>
@@ -8109,24 +8138,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EAC32C-8E28-4AF3-A227-0E5B0D99767C}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="37.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -8167,7 +8196,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30">
         <v>45642</v>
       </c>
@@ -8193,16 +8222,23 @@
         <f>IF(F2 &gt; 0, G2 * (F2 / 100), G2 * (100 / ABS(F2)))</f>
         <v>18.18181818181818</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
+      <c r="I2" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="26">
+        <f t="shared" ref="J2:J19" si="0">IF(I2="", "", IF(I2="Win", H2, -G2))</f>
+        <v>-20</v>
+      </c>
+      <c r="K2" s="25">
+        <v>7</v>
+      </c>
       <c r="L2" s="25"/>
       <c r="N2" s="3">
-        <f>SUM(J2:J30)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <f>SUM(J2:J29)</f>
+        <v>-53.228070175438589</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <v>45640</v>
       </c>
@@ -8225,15 +8261,18 @@
         <v>20</v>
       </c>
       <c r="H3" s="26">
-        <f t="shared" ref="H3:H4" si="0">IF(F3 &gt; 0, G3 * (F3 / 100), G3 * (100 / ABS(F3)))</f>
+        <f t="shared" ref="H3:H4" si="1">IF(F3 &gt; 0, G3 * (F3 / 100), G3 * (100 / ABS(F3)))</f>
         <v>19.047619047619047</v>
       </c>
       <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="J3" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K3" s="32"/>
       <c r="L3" s="32"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>45640</v>
       </c>
@@ -8256,15 +8295,18 @@
         <v>10</v>
       </c>
       <c r="H4" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0909090909090899</v>
       </c>
       <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
+      <c r="J4" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>45644</v>
       </c>
@@ -8287,15 +8329,18 @@
         <v>20</v>
       </c>
       <c r="H5" s="26">
-        <f t="shared" ref="H5:H12" si="1">IF(F5 &gt; 0, G5 * (F5 / 100), G5 * (100 / ABS(F5)))</f>
+        <f t="shared" ref="H5:H12" si="2">IF(F5 &gt; 0, G5 * (F5 / 100), G5 * (100 / ABS(F5)))</f>
         <v>40</v>
       </c>
       <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
+      <c r="J5" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>45643</v>
       </c>
@@ -8318,15 +8363,18 @@
         <v>20</v>
       </c>
       <c r="H6" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.18181818181818</v>
       </c>
       <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
+      <c r="J6" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>45643</v>
       </c>
@@ -8349,15 +8397,18 @@
         <v>49</v>
       </c>
       <c r="H7" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78.400000000000006</v>
       </c>
       <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
+      <c r="J7" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>45644</v>
       </c>
@@ -8380,15 +8431,18 @@
         <v>20</v>
       </c>
       <c r="H8" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.18181818181818</v>
       </c>
       <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
+      <c r="J8" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>45644</v>
       </c>
@@ -8411,15 +8465,22 @@
         <v>10</v>
       </c>
       <c r="H9" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0909090909090899</v>
       </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
+      <c r="I9" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="26">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="K9" s="25">
+        <v>61</v>
+      </c>
       <c r="L9" s="25"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30">
         <v>45644</v>
       </c>
@@ -8442,15 +8503,22 @@
         <v>10</v>
       </c>
       <c r="H10" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.695652173913043</v>
       </c>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
+      <c r="I10" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="26">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="K10" s="25">
+        <v>284</v>
+      </c>
       <c r="L10" s="25"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30">
         <v>45644</v>
       </c>
@@ -8473,15 +8541,22 @@
         <v>10</v>
       </c>
       <c r="H11" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.7719298245614024</v>
       </c>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
+      <c r="I11" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="26">
+        <f t="shared" si="0"/>
+        <v>8.7719298245614024</v>
+      </c>
+      <c r="K11" s="25">
+        <v>18</v>
+      </c>
       <c r="L11" s="25"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="31">
         <v>45644</v>
       </c>
@@ -8504,15 +8579,18 @@
         <v>20</v>
       </c>
       <c r="H12" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.18181818181818</v>
       </c>
       <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="J12" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K12" s="32"/>
       <c r="L12" s="32"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="30">
         <v>45644</v>
       </c>
@@ -8535,15 +8613,18 @@
         <v>5</v>
       </c>
       <c r="H13" s="26">
-        <f t="shared" ref="H13:H19" si="2">IF(F13 &gt; 0, G13 * (F13 / 100), G13 * (100 / ABS(F13)))</f>
+        <f t="shared" ref="H13:H19" si="3">IF(F13 &gt; 0, G13 * (F13 / 100), G13 * (100 / ABS(F13)))</f>
         <v>35</v>
       </c>
       <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
+      <c r="J13" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K13" s="25"/>
       <c r="L13" s="25"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="30">
         <v>45644</v>
       </c>
@@ -8566,15 +8647,18 @@
         <v>20</v>
       </c>
       <c r="H14" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.18181818181818</v>
       </c>
       <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
+      <c r="J14" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="30">
         <v>45644</v>
       </c>
@@ -8597,15 +8681,18 @@
         <v>20</v>
       </c>
       <c r="H15" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>181.81818181818184</v>
       </c>
       <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
+      <c r="J15" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K15" s="25"/>
       <c r="L15" s="25"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30">
         <v>45644</v>
       </c>
@@ -8628,15 +8715,22 @@
         <v>16.309999999999999</v>
       </c>
       <c r="H16" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20.387499999999999</v>
       </c>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
+      <c r="I16" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" s="26">
+        <f t="shared" si="0"/>
+        <v>-16.309999999999999</v>
+      </c>
+      <c r="K16" s="25">
+        <v>0</v>
+      </c>
       <c r="L16" s="25"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30">
         <v>45645</v>
       </c>
@@ -8659,47 +8753,156 @@
         <v>5.69</v>
       </c>
       <c r="H17" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102.42</v>
       </c>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
+      <c r="I17" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="26">
+        <f t="shared" si="0"/>
+        <v>-5.69</v>
+      </c>
+      <c r="K17" s="25">
+        <v>0</v>
+      </c>
       <c r="L17" s="25"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="30">
+        <v>45646</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="F18" s="25">
+        <v>-113</v>
+      </c>
+      <c r="G18" s="26">
+        <v>40</v>
+      </c>
+      <c r="H18" s="26">
+        <f t="shared" si="3"/>
+        <v>35.398230088495581</v>
       </c>
       <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
+      <c r="J18" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K18" s="25"/>
       <c r="L18" s="25"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="31">
+        <v>45646</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="F19" s="32">
+        <v>160</v>
+      </c>
+      <c r="G19" s="33">
+        <v>14.31</v>
+      </c>
+      <c r="H19" s="33">
+        <f t="shared" si="3"/>
+        <v>22.896000000000001</v>
       </c>
       <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
+      <c r="J19" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K19" s="32"/>
       <c r="L19" s="32"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="31">
+        <v>45647</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="F20" s="32">
+        <v>120</v>
+      </c>
+      <c r="G20" s="33">
+        <v>30</v>
+      </c>
+      <c r="H20" s="33">
+        <f>IF(F20 &gt; 0, G20 * (F20 / 100), G20 * (100 / ABS(F20)))</f>
+        <v>36</v>
+      </c>
+      <c r="I20" s="32"/>
+      <c r="J20" s="42" t="str">
+        <f>IF(I20="", "", IF(I20="Win", H20, -G20))</f>
+        <v/>
+      </c>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="30">
+        <v>45647</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="F21" s="25">
+        <v>833</v>
+      </c>
+      <c r="G21" s="26">
+        <v>5</v>
+      </c>
+      <c r="H21" s="26">
+        <f t="shared" ref="H21" si="4">IF(F21 &gt; 0, G21 * (F21 / 100), G21 * (100 / ABS(F21)))</f>
+        <v>41.65</v>
+      </c>
+      <c r="I21" s="25"/>
+      <c r="J21" s="41" t="str">
+        <f t="shared" ref="J21" si="5">IF(I21="", "", IF(I21="Win", H21, -G21))</f>
+        <v/>
+      </c>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8718,9 +8921,9 @@
       <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8761,7 +8964,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -8782,7 +8985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -8812,9 +9015,9 @@
       <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8855,7 +9058,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -8876,7 +9079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -8906,9 +9109,9 @@
       <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8949,7 +9152,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -8970,7 +9173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -9000,9 +9203,9 @@
       <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -9043,7 +9246,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -9064,7 +9267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -9094,9 +9297,9 @@
       <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -9137,7 +9340,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -9158,7 +9361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>

</xml_diff>